<commit_message>
Atualização de documentos. Correção de métricas no dashboard estático
</commit_message>
<xml_diff>
--- a/documentos/VISS_Matriz_Rastrabilidade.xlsx
+++ b/documentos/VISS_Matriz_Rastrabilidade.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Trabalhos\SPTech\2 semestre\PI\repos\viss\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B30997A-3425-429E-A036-81BC4CFC0B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B5742F6-4225-4E92-93EA-8E85656AEE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1031FC5E-348C-4BED-8817-77BF266A131C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{1031FC5E-348C-4BED-8817-77BF266A131C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="130">
   <si>
     <t>ID</t>
   </si>
@@ -208,7 +208,7 @@
   <si>
     <t>Tela de Relatórios da Equipe Técnica:    
 - Histogramas de uso de recursos de todos os equipamentos    
-- KPIs de quantidade de equipamentos comproblemas    
+- KPIs de quantidade de equipamentos com problemas    
 - Avisos    
 - Lista de Equipamentos</t>
   </si>
@@ -283,9 +283,6 @@
   </si>
   <si>
     <t>API NodeJS - Rota de Login</t>
-  </si>
-  <si>
-    <t>Rota de verificação de login, comparando informações com o que está presente na tabela Usuario</t>
   </si>
   <si>
     <t>API NodeJS - Rotas de dados dos relatórios</t>
@@ -351,16 +348,203 @@
 - Tela de Dashboard de Gerência</t>
   </si>
   <si>
+    <t>Helpdesk - Abertura automática de chamados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve abrir chamados automaticamente sempre que for registrado uma situação de alerta, como uso excessivo de recursos ou presença de programas maliciosos. </t>
+  </si>
+  <si>
     <t>Helpdesk - Integração com Slack</t>
   </si>
   <si>
     <t>Envio de mensagens automáticas após abertura de chamados, contendo descrição, número de protocolo e link para o chamado.</t>
   </si>
   <si>
-    <t>Helpdesk - Abertura automática de chamados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve abrir chamados automaticamente sempre que for registrado uma situação de alerta, como uso excessivo de recursos ou presença de programas maliciosos. </t>
+    <t>Aplicação Cliente - Rastreio de atividade</t>
+  </si>
+  <si>
+    <t>Cálculo de média de uso de teclado e mouse.</t>
+  </si>
+  <si>
+    <t>HelpDesk - Integração com formulário de contato</t>
+  </si>
+  <si>
+    <t>Abertura automática de chamado de solicitação de informação quando cliente utilizar o formulário de contato na página inicial</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Header contendo ícone da empresa e menu hamburger, com links para:
+- Login
+- Home (leva à seção chamada)
+- Sobre Nós
+- Serviços
+- Equipe
+- Contato</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>Chamada</t>
+  </si>
+  <si>
+    <t>Seção contendo imagem e slogan da empresa</t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t>Sobre Nós</t>
+  </si>
+  <si>
+    <t>Seção contendo valores da empresa, e objetivos que almejamos com nossos produtos e serviços.</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>Serviços</t>
+  </si>
+  <si>
+    <t>Seção contendo detalhes sobre o projeto V.I.S.S.</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>9.6</t>
+  </si>
+  <si>
+    <t>Equipe</t>
+  </si>
+  <si>
+    <t>Seção contendo nomes e fotos de integrantes da equipe</t>
+  </si>
+  <si>
+    <t>Contato</t>
+  </si>
+  <si>
+    <t>Formulário de contato, contendo campos para:
+- Nome
+- Email
+- Organização
+- Mensagem
+- Botão de envio</t>
+  </si>
+  <si>
+    <t>9.7</t>
+  </si>
+  <si>
+    <t>Rodapé</t>
+  </si>
+  <si>
+    <t>Rodapé da página, contendo links para mesmas seções presentes no menu hambúrguer, logo da empresa e informações de endereço e contato.</t>
+  </si>
+  <si>
+    <t>Tela de Relatórios Gerenciais:    
+- Histogramas de produtividade de funcionários    
+- KPIs de downtime e tempo médio de resolução de problemas
+- Avisos
+- Lista de funcionários</t>
+  </si>
+  <si>
+    <t>Diagrama detalhando principais atores e funcionalidades do sistema.</t>
+  </si>
+  <si>
+    <t>18.2</t>
+  </si>
+  <si>
+    <t>18.1</t>
+  </si>
+  <si>
+    <t>18.3</t>
+  </si>
+  <si>
+    <t>18.4</t>
+  </si>
+  <si>
+    <t>18.5</t>
+  </si>
+  <si>
+    <t>18.6</t>
+  </si>
+  <si>
+    <t>18.7</t>
+  </si>
+  <si>
+    <t>Leitura de dados de máquina, através de Python e Java:
+- CPU
+- RAM
+- Disco
+- Lista de processos
+- Uso de teclado e mouse</t>
+  </si>
+  <si>
+    <t>Rota de verificação de login, comparando informações de e-mail e senha com o que está presente na tabela Usuario</t>
+  </si>
+  <si>
+    <t>Tela de Relatórios da Equipe Técnica:    
+- Histogramas de uso de recursos de todos os equipamentos    
+- KPIs:
+    - Quantidade de equipamentos com problemas 
+    - Quantidade de equipamentos ligados
+- Alertas    
+- Lista de Equipamentos</t>
+  </si>
+  <si>
+    <t>Tela de Relatório Gerencial:    
+- KPIs:
+    - Downtime
+    - Jornada de trabalho.
+    - Atividade dos usuários
+- Lista de incidentes de uso de aplicações não desejáveis</t>
+  </si>
+  <si>
+    <t>Site Institucional - Carrosel de Imagens</t>
+  </si>
+  <si>
+    <t>Aplicação Cliente - Projeto Login Java</t>
+  </si>
+  <si>
+    <t>Sistema de login através de console, escrito em Java.
+Solicitação de nome e senha e comparação com dados mockados.
+Em caso de Login bem sucedido, libera uma função e opção de logout.</t>
+  </si>
+  <si>
+    <t>Implementação responsiva de carroseis de imagens nas páginas do Site:
+Home: Carrosel de Sobre Nós e Equipe.
+Dashboard: Carrosel dos gráficos de diferentes recursos.</t>
+  </si>
+  <si>
+    <t>Lista de Dados</t>
+  </si>
+  <si>
+    <t>Listagem dos dados que serão inseridos pelos usuários no sistema.</t>
+  </si>
+  <si>
+    <t>Desenho de fluxogramas de atendimento de chamados:
+- Fluxograma de Incidentes
+- Fluxograma de Problemas
+- Fluxograma de Solicitação</t>
+  </si>
+  <si>
+    <t>Criação de formulário de gestão de mudanças, Contendo:
+- Solicitante
+- Motivo da mudança
+- Processo de Implementação
+- Processo de Rollback
+- Janela de mudança
+- Aprovadores</t>
+  </si>
+  <si>
+    <t>Diagrama detalhando as classes existentes no sistema, seus respectivos atributos e métodos, envolvendo:
+- APIs de captura de dados;
+- Dashboards;</t>
   </si>
 </sst>
 </file>
@@ -384,12 +568,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -413,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,6 +624,15 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -744,15 +949,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BE498B-C80F-4373-8DDC-20BFC9A3A40B}">
-  <dimension ref="A1:Q178"/>
+  <dimension ref="A1:Q173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
@@ -797,7 +1003,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -828,7 +1034,7 @@
       <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -859,7 +1065,7 @@
       <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -890,7 +1096,7 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -921,7 +1127,7 @@
       <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -952,7 +1158,7 @@
       <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -983,7 +1189,7 @@
       <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1014,7 +1220,7 @@
       <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1045,7 +1251,7 @@
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1077,35 +1283,23 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:17" ht="345" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>10</v>
+    <row r="11" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="4">
-        <v>5</v>
-      </c>
-      <c r="G11" s="4">
-        <v>6</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="J11" s="5"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -1114,37 +1308,23 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="4">
-        <v>5</v>
-      </c>
-      <c r="G12" s="4">
-        <v>6</v>
-      </c>
-      <c r="H12" s="4">
-        <v>1</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -1153,37 +1333,23 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
     </row>
-    <row r="13" spans="1:17" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="4">
-        <v>8</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="4">
-        <v>1</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="5"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -1192,35 +1358,23 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>13</v>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="4">
-        <v>8</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="4">
-        <v>1</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>46</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
@@ -1229,25 +1383,19 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
+    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="4">
-        <v>5</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -1260,23 +1408,19 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>15</v>
+    <row r="16" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="4">
-        <v>8</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -1289,23 +1433,19 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>16</v>
+    <row r="17" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="4">
-        <v>13</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -1318,29 +1458,35 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>17</v>
+    <row r="18" spans="1:17" ht="345" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>10</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>52</v>
+        <v>32</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="4">
-        <v>8</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G18" s="4">
+        <v>6</v>
+      </c>
+      <c r="H18" s="4">
+        <v>1</v>
+      </c>
       <c r="I18" s="4"/>
-      <c r="J18" s="5"/>
+      <c r="J18" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -1349,31 +1495,37 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
     </row>
-    <row r="19" spans="1:17" ht="150" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>18</v>
+    <row r="19" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>11</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="4">
-        <v>13</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G19" s="4">
+        <v>6</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1</v>
+      </c>
       <c r="I19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
@@ -1382,18 +1534,18 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:17" ht="345" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>19</v>
+    <row r="20" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>13</v>
@@ -1401,15 +1553,17 @@
       <c r="F20" s="4">
         <v>8</v>
       </c>
-      <c r="G20" s="4">
-        <v>6</v>
+      <c r="G20" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="H20" s="4">
         <v>1</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="I20" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J20" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
@@ -1419,18 +1573,18 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
     </row>
-    <row r="21" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>20</v>
+    <row r="21" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>13</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>13</v>
@@ -1438,17 +1592,17 @@
       <c r="F21" s="4">
         <v>8</v>
       </c>
-      <c r="G21" s="4">
-        <v>6</v>
+      <c r="G21" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="H21" s="4">
         <v>1</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
@@ -1458,31 +1612,27 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>21</v>
+    <row r="22" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F22" s="4">
         <v>5</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H22" s="4">
-        <v>1</v>
-      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="4"/>
@@ -1493,35 +1643,29 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="1:17" ht="120" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>22</v>
+    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>15</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F23" s="4">
-        <v>13</v>
-      </c>
-      <c r="G23" s="4">
-        <v>6</v>
-      </c>
-      <c r="H23" s="4">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="J23" s="5"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -1530,35 +1674,29 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
     </row>
-    <row r="24" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>23</v>
+    <row r="24" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>16</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F24" s="4">
-        <v>8</v>
-      </c>
-      <c r="G24" s="4">
-        <v>6</v>
-      </c>
-      <c r="H24" s="4">
-        <v>1</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="J24" s="5"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -1567,14 +1705,16 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
     </row>
-    <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>24</v>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>17</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
       <c r="D25" s="4" t="s">
         <v>53</v>
       </c>
@@ -1582,18 +1722,12 @@
         <v>13</v>
       </c>
       <c r="F25" s="4">
-        <v>21</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" s="4">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="J25" s="5"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -1602,14 +1736,16 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
     </row>
-    <row r="26" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>25</v>
+    <row r="26" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>18</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="D26" s="4" t="s">
         <v>53</v>
       </c>
@@ -1619,18 +1755,12 @@
       <c r="F26" s="4">
         <v>13</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H26" s="4">
-        <v>1</v>
-      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
       <c r="I26" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="J26" s="5"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -1639,35 +1769,23 @@
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
     </row>
-    <row r="27" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>26</v>
+    <row r="27" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="4">
-        <v>13</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" s="4">
-        <v>1</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>46</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="5"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -1677,28 +1795,20 @@
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>27</v>
+      <c r="A28" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="4">
-        <v>21</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H28" s="4">
-        <v>1</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="5"/>
       <c r="K28" s="4"/>
@@ -1709,33 +1819,23 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>28</v>
+    <row r="29" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="4">
-        <v>8</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H29" s="4">
-        <v>1</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="J29" s="5"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
@@ -1744,37 +1844,23 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
     </row>
-    <row r="30" spans="1:17" ht="120" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>29</v>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="4">
-        <v>8</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H30" s="4">
-        <v>1</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="5"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -1783,23 +1869,19 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>30</v>
+    <row r="31" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="4">
-        <v>13</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
@@ -1812,23 +1894,19 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>31</v>
+    <row r="32" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" s="4">
-        <v>8</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
@@ -1841,23 +1919,19 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>32</v>
+    <row r="33" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="4">
-        <v>8</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -1870,29 +1944,35 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
     </row>
-    <row r="34" spans="1:17" ht="195" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+    <row r="34" spans="1:17" ht="345" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>19</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="D34" s="4" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F34" s="4">
         <v>8</v>
       </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="G34" s="4">
+        <v>6</v>
+      </c>
+      <c r="H34" s="4">
+        <v>1</v>
+      </c>
       <c r="I34" s="4"/>
-      <c r="J34" s="5"/>
+      <c r="J34" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -1902,28 +1982,36 @@
       <c r="Q34" s="4"/>
     </row>
     <row r="35" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>34</v>
+      <c r="A35" s="6">
+        <v>20</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F35" s="4">
-        <v>13</v>
-      </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="G35" s="4">
+        <v>6</v>
+      </c>
+      <c r="H35" s="4">
+        <v>1</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -1932,27 +2020,31 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
     </row>
-    <row r="36" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>35</v>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>21</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>81</v>
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>58</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F36" s="4">
-        <v>13</v>
-      </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H36" s="4">
+        <v>1</v>
+      </c>
       <c r="I36" s="4"/>
       <c r="J36" s="5"/>
       <c r="K36" s="4"/>
@@ -1963,14 +2055,35 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>36</v>
-      </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
+    <row r="37" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>22</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="4">
+        <v>13</v>
+      </c>
+      <c r="G37" s="4">
+        <v>6</v>
+      </c>
+      <c r="H37" s="4">
+        <v>1</v>
+      </c>
       <c r="I37" s="4"/>
-      <c r="J37" s="5"/>
+      <c r="J37" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -1979,19 +2092,35 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>37</v>
-      </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
+    <row r="38" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>23</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="4">
+        <v>8</v>
+      </c>
+      <c r="G38" s="4">
+        <v>6</v>
+      </c>
+      <c r="H38" s="4">
+        <v>1</v>
+      </c>
       <c r="I38" s="4"/>
-      <c r="J38" s="5"/>
+      <c r="J38" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
@@ -2000,19 +2129,33 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>38</v>
-      </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
+    <row r="39" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>24</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="4">
+        <v>21</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="4">
+        <v>1</v>
+      </c>
       <c r="I39" s="4"/>
-      <c r="J39" s="5"/>
+      <c r="J39" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -2021,19 +2164,37 @@
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
-        <v>39</v>
-      </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="5"/>
+    <row r="40" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>25</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="4">
+        <v>13</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H40" s="4">
+        <v>1</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -2042,19 +2203,37 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <v>40</v>
-      </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="5"/>
+    <row r="41" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>26</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="4">
+        <v>13</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H41" s="4">
+        <v>1</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -2063,17 +2242,31 @@
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>41</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
+    <row r="42" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>27</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="4">
+        <v>21</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1</v>
+      </c>
       <c r="I42" s="4"/>
       <c r="J42" s="5"/>
       <c r="K42" s="4"/>
@@ -2085,18 +2278,32 @@
       <c r="Q42" s="4"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
-        <v>42</v>
-      </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
+      <c r="A43" s="7">
+        <v>28</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="4">
+        <v>8</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H43" s="4">
+        <v>1</v>
+      </c>
       <c r="I43" s="4"/>
-      <c r="J43" s="5"/>
+      <c r="J43" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
@@ -2105,19 +2312,37 @@
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+    <row r="44" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>29</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="4">
+        <v>8</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H44" s="4">
+        <v>1</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J44" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="5"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
@@ -2126,15 +2351,25 @@
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
-        <v>44</v>
-      </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
+    <row r="45" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>30</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" s="4">
+        <v>13</v>
+      </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
@@ -2147,15 +2382,25 @@
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>45</v>
-      </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
+    <row r="46" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>31</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" s="4">
+        <v>8</v>
+      </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
@@ -2169,14 +2414,22 @@
       <c r="Q46" s="4"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>46</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
+      <c r="A47" s="6">
+        <v>32</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="4">
+        <v>8</v>
+      </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
@@ -2189,841 +2442,887 @@
       <c r="P47" s="4"/>
       <c r="Q47" s="4"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="G48" s="3"/>
-      <c r="J48" s="2"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="G49" s="3"/>
-      <c r="J49" s="2"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="G50" s="3"/>
-      <c r="J50" s="2"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="G51" s="3"/>
-      <c r="J51" s="2"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="G52" s="3"/>
-      <c r="J52" s="2"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="C53" s="2"/>
-      <c r="G53" s="3"/>
-      <c r="J53" s="2"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="48" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>33</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="4">
+        <v>8</v>
+      </c>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+    </row>
+    <row r="49" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>34</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="2"/>
-      <c r="G54" s="3"/>
-      <c r="J54" s="2"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="G55" s="3"/>
-      <c r="J55" s="2"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="C56" s="2"/>
-      <c r="G56" s="3"/>
-      <c r="J56" s="2"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="C57" s="2"/>
-      <c r="G57" s="3"/>
-      <c r="J57" s="2"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="G58" s="3"/>
-      <c r="J58" s="2"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="G59" s="3"/>
-      <c r="J59" s="2"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="C60" s="2"/>
-      <c r="J60" s="2"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="J61" s="2"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>61</v>
-      </c>
+      <c r="E49" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="4">
+        <v>13</v>
+      </c>
+      <c r="G49" s="4">
+        <v>7</v>
+      </c>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+    </row>
+    <row r="50" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>35</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="4">
+        <v>13</v>
+      </c>
+      <c r="G50" s="4">
+        <v>7</v>
+      </c>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>36</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="4">
+        <v>13</v>
+      </c>
+      <c r="G51" s="4">
+        <v>8</v>
+      </c>
+      <c r="H51" s="4">
+        <v>1</v>
+      </c>
+      <c r="I51" s="4"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+    </row>
+    <row r="52" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>37</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="4">
+        <v>5</v>
+      </c>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+    </row>
+    <row r="53" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>38</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" s="4">
+        <v>21</v>
+      </c>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+    </row>
+    <row r="54" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>39</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="4">
+        <v>13</v>
+      </c>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+    </row>
+    <row r="55" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>40</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="4">
+        <v>5</v>
+      </c>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="6"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="4"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" s="6"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
       <c r="C62" s="2"/>
+      <c r="G62" s="3"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>62</v>
-      </c>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
       <c r="C63" s="2"/>
+      <c r="G63" s="3"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>63</v>
-      </c>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
       <c r="C64" s="2"/>
+      <c r="G64" s="3"/>
       <c r="J64" s="2"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>64</v>
-      </c>
+      <c r="A65" s="3"/>
       <c r="C65" s="2"/>
+      <c r="G65" s="3"/>
       <c r="J65" s="2"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>65</v>
-      </c>
+      <c r="A66" s="3"/>
       <c r="C66" s="2"/>
+      <c r="G66" s="3"/>
       <c r="J66" s="2"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>66</v>
-      </c>
+      <c r="A67" s="3"/>
       <c r="C67" s="2"/>
+      <c r="G67" s="3"/>
       <c r="J67" s="2"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>67</v>
-      </c>
+      <c r="A68" s="3"/>
       <c r="C68" s="2"/>
+      <c r="G68" s="3"/>
       <c r="J68" s="2"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>68</v>
-      </c>
+      <c r="A69" s="3"/>
       <c r="C69" s="2"/>
+      <c r="G69" s="3"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>69</v>
-      </c>
+      <c r="A70" s="3"/>
       <c r="C70" s="2"/>
+      <c r="G70" s="3"/>
       <c r="J70" s="2"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>70</v>
-      </c>
+      <c r="A71" s="3"/>
       <c r="C71" s="2"/>
+      <c r="G71" s="3"/>
       <c r="J71" s="2"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>71</v>
-      </c>
+      <c r="A72" s="3"/>
       <c r="C72" s="2"/>
+      <c r="G72" s="3"/>
       <c r="J72" s="2"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>72</v>
-      </c>
+      <c r="A73" s="3"/>
       <c r="C73" s="2"/>
+      <c r="G73" s="3"/>
       <c r="J73" s="2"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>73</v>
-      </c>
+      <c r="A74" s="3"/>
       <c r="C74" s="2"/>
       <c r="J74" s="2"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>74</v>
-      </c>
+      <c r="A75" s="3"/>
       <c r="C75" s="2"/>
       <c r="J75" s="2"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>75</v>
-      </c>
+      <c r="A76" s="3"/>
       <c r="C76" s="2"/>
       <c r="J76" s="2"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>76</v>
-      </c>
+      <c r="A77" s="3"/>
       <c r="C77" s="2"/>
       <c r="J77" s="2"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>77</v>
-      </c>
+      <c r="A78" s="3"/>
       <c r="C78" s="2"/>
       <c r="J78" s="2"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>78</v>
-      </c>
+      <c r="A79" s="3"/>
       <c r="C79" s="2"/>
       <c r="J79" s="2"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>79</v>
-      </c>
+      <c r="A80" s="3"/>
       <c r="C80" s="2"/>
       <c r="J80" s="2"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>80</v>
-      </c>
+      <c r="A81" s="3"/>
       <c r="C81" s="2"/>
       <c r="J81" s="2"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>81</v>
-      </c>
+      <c r="A82" s="3"/>
       <c r="C82" s="2"/>
       <c r="J82" s="2"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>82</v>
-      </c>
+      <c r="A83" s="3"/>
       <c r="C83" s="2"/>
       <c r="J83" s="2"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>83</v>
-      </c>
+      <c r="A84" s="3"/>
       <c r="C84" s="2"/>
       <c r="J84" s="2"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>84</v>
-      </c>
+      <c r="A85" s="3"/>
       <c r="C85" s="2"/>
       <c r="J85" s="2"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>85</v>
-      </c>
+      <c r="A86" s="3"/>
       <c r="C86" s="2"/>
       <c r="J86" s="2"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>86</v>
-      </c>
+      <c r="A87" s="3"/>
       <c r="C87" s="2"/>
       <c r="J87" s="2"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>87</v>
-      </c>
+      <c r="A88" s="3"/>
       <c r="C88" s="2"/>
       <c r="J88" s="2"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>88</v>
-      </c>
+      <c r="A89" s="3"/>
       <c r="C89" s="2"/>
       <c r="J89" s="2"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>89</v>
-      </c>
+      <c r="A90" s="3"/>
       <c r="C90" s="2"/>
       <c r="J90" s="2"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>90</v>
-      </c>
+      <c r="A91" s="3"/>
       <c r="C91" s="2"/>
       <c r="J91" s="2"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>91</v>
-      </c>
+      <c r="A92" s="3"/>
       <c r="C92" s="2"/>
       <c r="J92" s="2"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>92</v>
-      </c>
+      <c r="A93" s="3"/>
       <c r="C93" s="2"/>
       <c r="J93" s="2"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>93</v>
-      </c>
+      <c r="A94" s="3"/>
       <c r="C94" s="2"/>
       <c r="J94" s="2"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>94</v>
-      </c>
+      <c r="A95" s="3"/>
       <c r="C95" s="2"/>
       <c r="J95" s="2"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>95</v>
-      </c>
+      <c r="A96" s="3"/>
       <c r="C96" s="2"/>
       <c r="J96" s="2"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>96</v>
-      </c>
+      <c r="A97" s="3"/>
       <c r="C97" s="2"/>
       <c r="J97" s="2"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>97</v>
-      </c>
+      <c r="A98" s="3"/>
       <c r="C98" s="2"/>
       <c r="J98" s="2"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>98</v>
-      </c>
+      <c r="A99" s="3"/>
       <c r="C99" s="2"/>
       <c r="J99" s="2"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>99</v>
-      </c>
+      <c r="A100" s="3"/>
       <c r="C100" s="2"/>
       <c r="J100" s="2"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>100</v>
-      </c>
+      <c r="A101" s="3"/>
       <c r="C101" s="2"/>
       <c r="J101" s="2"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>101</v>
-      </c>
+      <c r="A102" s="3"/>
       <c r="C102" s="2"/>
       <c r="J102" s="2"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>102</v>
-      </c>
+      <c r="A103" s="3"/>
       <c r="C103" s="2"/>
       <c r="J103" s="2"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>103</v>
-      </c>
+      <c r="A104" s="3"/>
       <c r="C104" s="2"/>
       <c r="J104" s="2"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <v>104</v>
-      </c>
+      <c r="A105" s="3"/>
+      <c r="C105" s="2"/>
       <c r="J105" s="2"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106">
-        <v>105</v>
-      </c>
+      <c r="A106" s="3"/>
+      <c r="C106" s="2"/>
       <c r="J106" s="2"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107">
-        <v>106</v>
-      </c>
+      <c r="A107" s="3"/>
+      <c r="C107" s="2"/>
       <c r="J107" s="2"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108">
-        <v>107</v>
-      </c>
+      <c r="A108" s="3"/>
+      <c r="C108" s="2"/>
       <c r="J108" s="2"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109">
-        <v>108</v>
-      </c>
+      <c r="A109" s="3"/>
+      <c r="C109" s="2"/>
       <c r="J109" s="2"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110">
-        <v>109</v>
-      </c>
+      <c r="A110" s="3"/>
+      <c r="C110" s="2"/>
       <c r="J110" s="2"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111">
-        <v>110</v>
-      </c>
+      <c r="A111" s="3"/>
+      <c r="C111" s="2"/>
       <c r="J111" s="2"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112">
-        <v>111</v>
-      </c>
+      <c r="A112" s="3"/>
+      <c r="C112" s="2"/>
       <c r="J112" s="2"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113">
-        <v>112</v>
-      </c>
+      <c r="A113" s="3"/>
+      <c r="C113" s="2"/>
       <c r="J113" s="2"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>113</v>
-      </c>
+      <c r="A114" s="3"/>
+      <c r="C114" s="2"/>
       <c r="J114" s="2"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>114</v>
-      </c>
+      <c r="A115" s="3"/>
+      <c r="C115" s="2"/>
       <c r="J115" s="2"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116">
-        <v>115</v>
-      </c>
+      <c r="A116" s="3"/>
+      <c r="C116" s="2"/>
       <c r="J116" s="2"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117">
-        <v>116</v>
-      </c>
+      <c r="A117" s="3"/>
+      <c r="C117" s="2"/>
       <c r="J117" s="2"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <v>117</v>
-      </c>
+      <c r="A118" s="3"/>
+      <c r="C118" s="2"/>
       <c r="J118" s="2"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>118</v>
-      </c>
+      <c r="A119" s="3"/>
       <c r="J119" s="2"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>119</v>
-      </c>
+      <c r="A120" s="3"/>
       <c r="J120" s="2"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121">
-        <v>120</v>
-      </c>
+      <c r="A121" s="3"/>
       <c r="J121" s="2"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122">
-        <v>121</v>
-      </c>
+      <c r="A122" s="3"/>
       <c r="J122" s="2"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123">
-        <v>122</v>
-      </c>
+      <c r="A123" s="3"/>
       <c r="J123" s="2"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124">
-        <v>123</v>
-      </c>
+      <c r="A124" s="3"/>
       <c r="J124" s="2"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125">
-        <v>124</v>
-      </c>
+      <c r="A125" s="3"/>
       <c r="J125" s="2"/>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A126">
-        <v>125</v>
-      </c>
+      <c r="A126" s="3"/>
       <c r="J126" s="2"/>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A127">
-        <v>126</v>
-      </c>
+      <c r="A127" s="3"/>
       <c r="J127" s="2"/>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A128">
-        <v>127</v>
-      </c>
+      <c r="A128" s="3"/>
       <c r="J128" s="2"/>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A129">
-        <v>128</v>
-      </c>
+      <c r="A129" s="3"/>
       <c r="J129" s="2"/>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A130">
-        <v>129</v>
-      </c>
+      <c r="A130" s="3"/>
       <c r="J130" s="2"/>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A131">
-        <v>130</v>
-      </c>
+      <c r="A131" s="3"/>
       <c r="J131" s="2"/>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A132">
-        <v>131</v>
-      </c>
+      <c r="A132" s="3"/>
       <c r="J132" s="2"/>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A133">
-        <v>132</v>
-      </c>
+      <c r="A133" s="3"/>
       <c r="J133" s="2"/>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A134">
-        <v>133</v>
-      </c>
+      <c r="A134" s="3"/>
       <c r="J134" s="2"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A135">
-        <v>134</v>
-      </c>
+      <c r="A135" s="3"/>
       <c r="J135" s="2"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A136">
-        <v>135</v>
-      </c>
+      <c r="A136" s="3"/>
       <c r="J136" s="2"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137">
-        <v>136</v>
-      </c>
+      <c r="A137" s="3"/>
       <c r="J137" s="2"/>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A138">
-        <v>137</v>
-      </c>
+      <c r="A138" s="3"/>
       <c r="J138" s="2"/>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A139">
-        <v>138</v>
-      </c>
+      <c r="A139" s="3"/>
       <c r="J139" s="2"/>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A140">
-        <v>139</v>
-      </c>
+      <c r="A140" s="3"/>
       <c r="J140" s="2"/>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A141">
-        <v>140</v>
-      </c>
+      <c r="A141" s="3"/>
       <c r="J141" s="2"/>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A142">
-        <v>141</v>
-      </c>
+      <c r="A142" s="3"/>
       <c r="J142" s="2"/>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A143">
-        <v>142</v>
-      </c>
+      <c r="A143" s="3"/>
       <c r="J143" s="2"/>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <v>143</v>
-      </c>
+      <c r="A144" s="3"/>
       <c r="J144" s="2"/>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A145">
-        <v>144</v>
-      </c>
+      <c r="A145" s="3"/>
       <c r="J145" s="2"/>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <v>145</v>
-      </c>
+      <c r="A146" s="3"/>
       <c r="J146" s="2"/>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <v>146</v>
-      </c>
+      <c r="A147" s="3"/>
       <c r="J147" s="2"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A148">
-        <v>147</v>
-      </c>
+      <c r="A148" s="3"/>
       <c r="J148" s="2"/>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A149">
-        <v>148</v>
-      </c>
+      <c r="A149" s="3"/>
       <c r="J149" s="2"/>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A150">
-        <v>149</v>
-      </c>
+      <c r="A150" s="3"/>
       <c r="J150" s="2"/>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A151">
-        <v>150</v>
-      </c>
+      <c r="A151" s="3"/>
       <c r="J151" s="2"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A152">
-        <v>151</v>
-      </c>
+      <c r="A152" s="3"/>
       <c r="J152" s="2"/>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A153">
-        <v>152</v>
-      </c>
+      <c r="A153" s="3"/>
       <c r="J153" s="2"/>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A154">
-        <v>153</v>
-      </c>
+      <c r="A154" s="3"/>
       <c r="J154" s="2"/>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A155">
-        <v>154</v>
-      </c>
+      <c r="A155" s="3"/>
       <c r="J155" s="2"/>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A156">
-        <v>155</v>
-      </c>
+      <c r="A156" s="3"/>
       <c r="J156" s="2"/>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A157">
-        <v>156</v>
-      </c>
+      <c r="A157" s="3"/>
       <c r="J157" s="2"/>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A158">
-        <v>157</v>
-      </c>
+      <c r="A158" s="3"/>
       <c r="J158" s="2"/>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A159">
-        <v>158</v>
-      </c>
+      <c r="A159" s="3"/>
       <c r="J159" s="2"/>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A160">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178">
-        <v>177</v>
-      </c>
+      <c r="A160" s="3"/>
+      <c r="J160" s="2"/>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161" s="3"/>
+      <c r="J161" s="2"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162" s="3"/>
+      <c r="J162" s="2"/>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" s="3"/>
+      <c r="J163" s="2"/>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" s="3"/>
+      <c r="J164" s="2"/>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A165" s="3"/>
+      <c r="J165" s="2"/>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A166" s="3"/>
+      <c r="J166" s="2"/>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167" s="3"/>
+      <c r="J167" s="2"/>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168" s="3"/>
+      <c r="J168" s="2"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J169" s="2"/>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J170" s="2"/>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J171" s="2"/>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J172" s="2"/>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J173" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3031,14 +3330,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="58bd19be-68b1-440c-82af-6d4de24fec6c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003236BA383373F9498A6F9C22979A1745" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="105d9e49bcf5018a2b9f673ffb6bea80">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="58bd19be-68b1-440c-82af-6d4de24fec6c" xmlns:ns4="3ffc9a63-5890-437d-bab6-67d84705b086" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d014951b45a5d9b1402ae11632260839" ns3:_="" ns4:_="">
     <xsd:import namespace="58bd19be-68b1-440c-82af-6d4de24fec6c"/>
@@ -3227,6 +3518,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="58bd19be-68b1-440c-82af-6d4de24fec6c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3237,23 +3536,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E86881A-F23D-4E3F-AE75-8C4019D8C552}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="58bd19be-68b1-440c-82af-6d4de24fec6c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3ffc9a63-5890-437d-bab6-67d84705b086"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE152437-BE8E-4CC8-8716-2E0AF15B3C02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3272,6 +3554,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E86881A-F23D-4E3F-AE75-8C4019D8C552}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="58bd19be-68b1-440c-82af-6d4de24fec6c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3ffc9a63-5890-437d-bab6-67d84705b086"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C00E1856-A5B8-4D36-B8FD-2DB6EDAEB375}">
   <ds:schemaRefs>

</xml_diff>